<commit_message>
add extra parts disclaimer
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\roachslimes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57967C02-DCEE-4FF8-9348-D6FF1F8FC79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC697079-C2AF-468F-8000-891C2CBE73CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21390" xr2:uid="{AB7D66DD-99DB-4E79-8386-D1BE3E306A87}"/>
   </bookViews>
@@ -1769,7 +1769,7 @@
   <dimension ref="A1:AA45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AN14" sqref="AN14"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1903,10 +1903,7 @@
       <c r="P2" s="2">
         <v>2</v>
       </c>
-      <c r="Q2" s="3">
-        <f>SUM(B2:P2)</f>
-        <v>71.77</v>
-      </c>
+      <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1967,63 +1964,63 @@
         <v>33</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:P4" si="0">SUM(B2*B7,B3)</f>
+        <f>SUM(B2*B7,B3)</f>
         <v>15.5</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(C2*C7,C3)</f>
         <v>12.88</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(D2*D7,D3)</f>
         <v>3.27</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(E2*E7,E3)</f>
         <v>6.9599999999999991</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(F2*F7,F3)</f>
         <v>1.2</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(G2*G7,G3)</f>
         <v>3.79</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(H2*H7,H3)</f>
         <v>12.93</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(I2*I7,I3)</f>
         <v>1.2</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(J2*J7,J3)</f>
         <v>1.05</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(K2*K7,K3)</f>
         <v>1.05</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(L2*L7,L3)</f>
         <v>2.4700000000000002</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(M2*M7,M3)</f>
         <v>25.99</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(N2*N7,N3)</f>
         <v>11.93</v>
       </c>
       <c r="O4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(O2*O7,O3)</f>
         <v>3.52</v>
       </c>
       <c r="P4" s="2">
-        <f t="shared" si="0"/>
+        <f>SUM(P2*P7,P3)</f>
         <v>3.52</v>
       </c>
       <c r="Q4" s="3">
@@ -2115,59 +2112,59 @@
         <v>16.778749999999999</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" ref="C6:P6" si="1">SUM(C5,C4)</f>
+        <f t="shared" ref="C6:P6" si="0">SUM(C5,C4)</f>
         <v>13.942600000000001</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.5397750000000001</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7.5341999999999993</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2989999999999999</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.1026749999999996</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" ref="H6" si="2">SUM(H5,H4)</f>
+        <f t="shared" ref="H6" si="1">SUM(H5,H4)</f>
         <v>13.996725</v>
       </c>
       <c r="I6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2989999999999999</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.136625</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" ref="K6" si="3">SUM(K5,K4)</f>
+        <f t="shared" ref="K6" si="2">SUM(K5,K4)</f>
         <v>1.136625</v>
       </c>
       <c r="L6" s="3">
-        <f t="shared" ref="L6" si="4">SUM(L5,L4)</f>
+        <f t="shared" ref="L6" si="3">SUM(L5,L4)</f>
         <v>2.673775</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28.134174999999999</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12.914225</v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.8104</v>
       </c>
       <c r="P6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.8104</v>
       </c>
       <c r="Q6" s="3">
@@ -2322,63 +2319,63 @@
         <v>3</v>
       </c>
       <c r="B9" s="3">
-        <f t="shared" ref="B9:P9" si="5">(B6/B7)/B8</f>
+        <f>(B6/B7)/B8</f>
         <v>1.8643055555555554</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="5"/>
+        <f>(C6/C7)/C8</f>
         <v>1.1618833333333334</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="5"/>
+        <f>(D6/D7)/D8</f>
         <v>0.17698875</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="5"/>
+        <f>(E6/E7)/E8</f>
         <v>0.62784999999999991</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="5"/>
+        <f>(F6/F7)/F8</f>
         <v>6.4949999999999994E-2</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="5"/>
+        <f>(G6/G7)/G8</f>
         <v>4.1026749999999994E-2</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="5"/>
+        <f>(H6/H7)/H8</f>
         <v>0.69983624999999994</v>
       </c>
       <c r="I9" s="3">
-        <f t="shared" si="5"/>
+        <f>(I6/I7)/I8</f>
         <v>1.299E-2</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="5"/>
+        <f>(J6/J7)/J8</f>
         <v>1.136625E-2</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="5"/>
+        <f>(K6/K7)/K8</f>
         <v>1.136625E-2</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="5"/>
+        <f>(L6/L7)/L8</f>
         <v>4.4562916666666666E-3</v>
       </c>
       <c r="M9" s="3">
-        <f t="shared" si="5"/>
+        <f>(M6/M7)/M8</f>
         <v>2.8134174999999999</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" si="5"/>
+        <f>(N6/N7)/N8</f>
         <v>1.0761854166666667</v>
       </c>
       <c r="O9" s="3">
-        <f t="shared" si="5"/>
+        <f>(O6/O7)/O8</f>
         <v>0.19051999999999999</v>
       </c>
       <c r="P9" s="3">
-        <f t="shared" si="5"/>
+        <f>(P6/P7)/P8</f>
         <v>9.5259999999999997E-2</v>
       </c>
       <c r="Q9" s="3"/>
@@ -2579,47 +2576,47 @@
         <v>1.8643055555555554</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" ref="C14:P14" si="6">C9*C11</f>
+        <f t="shared" ref="C14:P14" si="4">C9*C11</f>
         <v>1.1618833333333334</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.17698875</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.62784999999999991</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>6.4949999999999994E-2</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.1026749999999994E-2</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" ref="H14" si="7">H9*H11</f>
+        <f t="shared" ref="H14" si="5">H9*H11</f>
         <v>0.69983624999999994</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.598E-2</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.136625E-2</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" ref="K14" si="8">K9*K11</f>
+        <f t="shared" ref="K14" si="6">K9*K11</f>
         <v>1.136625E-2</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" ref="L14" si="9">L9*L11</f>
+        <f t="shared" ref="L14" si="7">L9*L11</f>
         <v>4.4562916666666666E-3</v>
       </c>
       <c r="M14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.8134174999999999</v>
       </c>
       <c r="N14" s="3">
@@ -2627,11 +2624,11 @@
         <v>0</v>
       </c>
       <c r="O14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.19051999999999999</v>
       </c>
       <c r="P14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q14" s="3">
@@ -2671,59 +2668,59 @@
         <v>0</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" ref="C15:P15" si="10">C9*C12</f>
+        <f t="shared" ref="C15:P15" si="8">C9*C12</f>
         <v>1.1618833333333334</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0.62784999999999991</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>4.1026749999999994E-2</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" ref="H15" si="11">H9*H12</f>
+        <f t="shared" ref="H15" si="9">H9*H12</f>
         <v>0</v>
       </c>
       <c r="I15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" ref="K15" si="12">K9*K12</f>
+        <f t="shared" ref="K15" si="10">K9*K12</f>
         <v>0</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" ref="L15" si="13">L9*L12</f>
+        <f t="shared" ref="L15" si="11">L9*L12</f>
         <v>0</v>
       </c>
       <c r="M15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" ref="N15" si="14">N9*N12</f>
+        <f t="shared" ref="N15" si="12">N9*N12</f>
         <v>1.0761854166666667</v>
       </c>
       <c r="O15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9.5259999999999997E-2</v>
       </c>
       <c r="Q15" s="3">
@@ -2974,7 +2971,7 @@
         <v>13</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" ref="B24" si="15">SUM(B23,B22)</f>
+        <f t="shared" ref="B24" si="13">SUM(B23,B22)</f>
         <v>6.6249000000000002</v>
       </c>
       <c r="C24" s="3">
@@ -3030,15 +3027,15 @@
         <v>55</v>
       </c>
       <c r="U25" s="9">
-        <f t="shared" ref="U25:W25" si="16">SUM(U23:U24)</f>
+        <f t="shared" ref="U25:W25" si="14">SUM(U23:U24)</f>
         <v>58.666666666666664</v>
       </c>
       <c r="V25" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>66</v>
       </c>
       <c r="W25" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>88</v>
       </c>
       <c r="X25" s="9">
@@ -3257,19 +3254,19 @@
         <v>8.714125000000001</v>
       </c>
       <c r="U33" s="3">
-        <f t="shared" ref="U33:X33" si="17">SUM(U30:U31)</f>
+        <f t="shared" ref="U33:X33" si="15">SUM(U30:U31)</f>
         <v>8.714125000000001</v>
       </c>
       <c r="V33" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>8.714125000000001</v>
       </c>
       <c r="W33" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>8.714125000000001</v>
       </c>
       <c r="X33" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>8.714125000000001</v>
       </c>
     </row>
@@ -3327,19 +3324,19 @@
         <v>106.96417965277777</v>
       </c>
       <c r="U35" s="3">
-        <f t="shared" ref="U35:X35" si="18">SUM(U33,U27)</f>
+        <f t="shared" ref="U35:X35" si="16">SUM(U33,U27)</f>
         <v>115.22649181944445</v>
       </c>
       <c r="V35" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>129.88921615277778</v>
       </c>
       <c r="W35" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>168.8705500138889</v>
       </c>
       <c r="X35" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>244.95900730555556</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added r1 case files
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\roachslimes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC697079-C2AF-468F-8000-891C2CBE73CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9F0BDE-7969-4E3A-AA52-2B5E1857537E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21390" xr2:uid="{AB7D66DD-99DB-4E79-8386-D1BE3E306A87}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21150" xr2:uid="{AB7D66DD-99DB-4E79-8386-D1BE3E306A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,6 +457,148 @@
   </cellStyles>
   <dxfs count="59">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
@@ -992,148 +1134,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1327,51 +1327,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B14A7224-19B0-4C1A-A967-E81C81040A40}" name="Table1" displayName="Table1" ref="A1:Q17" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B14A7224-19B0-4C1A-A967-E81C81040A40}" name="Table1" displayName="Table1" ref="A1:Q17" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:Q17" xr:uid="{B14A7224-19B0-4C1A-A967-E81C81040A40}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{FCE3FD92-4E2D-4CDD-8748-B2B792C3CC2B}" name=" Tracker Components" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{C043608B-6B21-430A-A486-3DBF4D729827}" name="D1 Mini" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{0FD903D3-5CF3-4816-A12C-6B81AD38D598}" name="BMI160" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{AF1B510F-1F13-4EBF-9516-C6875CCCE2FD}" name="TP4056" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{EDED6859-BC93-4D0F-9315-A40F96119E83}" name="GY-271" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{7FD415BD-A930-4596-BA13-FDA67B16B7F4}" name="SK12D07VG4 " dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{A90A17C3-9B69-4679-A66B-0EDE0EB27F40}" name="JST-PH-4P" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{FCE3FD92-4E2D-4CDD-8748-B2B792C3CC2B}" name=" Tracker Components" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{C043608B-6B21-430A-A486-3DBF4D729827}" name="D1 Mini" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{0FD903D3-5CF3-4816-A12C-6B81AD38D598}" name="BMI160" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{AF1B510F-1F13-4EBF-9516-C6875CCCE2FD}" name="TP4056" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{EDED6859-BC93-4D0F-9315-A40F96119E83}" name="GY-271" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{7FD415BD-A930-4596-BA13-FDA67B16B7F4}" name="SK12D07VG4 " dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{A90A17C3-9B69-4679-A66B-0EDE0EB27F40}" name="JST-PH-4P" dataDxfId="7"/>
     <tableColumn id="20" xr3:uid="{BB4AB17F-F072-4577-B885-41BCCBC80B3B}" name="Pogo Female"/>
-    <tableColumn id="8" xr3:uid="{A914F9A6-5FD6-48EC-9D66-948BA78CA99E}" name="B5817WS" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{38CC02EE-7A21-4150-81A5-541E2C9611DA}" name="0805 180k" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{A914F9A6-5FD6-48EC-9D66-948BA78CA99E}" name="B5817WS" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{38CC02EE-7A21-4150-81A5-541E2C9611DA}" name="0805 180k" dataDxfId="5"/>
     <tableColumn id="17" xr3:uid="{D06AA3FD-469E-44E7-954C-59BA219B5A1D}" name="0806 620r"/>
     <tableColumn id="18" xr3:uid="{A346B222-7458-4A1F-8FDB-BE9A824753D5}" name="0805 LED"/>
-    <tableColumn id="10" xr3:uid="{F09ECC99-91ED-41A2-B73F-32BA143514AC}" name="803450" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{D2F40E9F-6B6D-42C4-81A7-8C00F83ACB72}" name="Wires" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{1CAFA1EE-4F95-4300-8E25-43760021F16D}" name="Motherboard" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{EBB820E5-8589-4BC4-925B-FE2B3CF62FFC}" name="Daughterboard" dataDxfId="44"/>
-    <tableColumn id="14" xr3:uid="{A324B42F-BFC5-4670-BD72-3FF95C7E905F}" name="Total" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{F09ECC99-91ED-41A2-B73F-32BA143514AC}" name="803450" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{D2F40E9F-6B6D-42C4-81A7-8C00F83ACB72}" name="Wires" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{1CAFA1EE-4F95-4300-8E25-43760021F16D}" name="Motherboard" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{EBB820E5-8589-4BC4-925B-FE2B3CF62FFC}" name="Daughterboard" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{A324B42F-BFC5-4670-BD72-3FF95C7E905F}" name="Total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B93392DA-EFC7-40A8-935E-E4659A1D9845}" name="Table2" displayName="Table2" ref="S7:X20" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B93392DA-EFC7-40A8-935E-E4659A1D9845}" name="Table2" displayName="Table2" ref="S7:X20" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="S7:X20" xr:uid="{B93392DA-EFC7-40A8-935E-E4659A1D9845}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B05F922E-1AED-4BDF-AF79-C73D0E339E8C}" name=" Materials Cost" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{890D8999-0321-4F67-A5E0-25676EB95AFA}" name="Lower Body Set" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{965D71D9-87D7-40F0-AB78-E63CEFFF194C}" name="Core Set" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{A87423F7-0BA3-4F6A-B4AF-D56080DE192B}" name="Enhanced Core Set" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{15F82D2F-735C-4D15-9CD1-2FFAC68D783A}" name="Full Body Set" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{268904B6-4873-466C-AF49-A18E0B9EB3F6}" name="Deluxe Tracker Set" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{B05F922E-1AED-4BDF-AF79-C73D0E339E8C}" name=" Materials Cost" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{890D8999-0321-4F67-A5E0-25676EB95AFA}" name="Lower Body Set" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{965D71D9-87D7-40F0-AB78-E63CEFFF194C}" name="Core Set" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{A87423F7-0BA3-4F6A-B4AF-D56080DE192B}" name="Enhanced Core Set" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{15F82D2F-735C-4D15-9CD1-2FFAC68D783A}" name="Full Body Set" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{268904B6-4873-466C-AF49-A18E0B9EB3F6}" name="Deluxe Tracker Set" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B9449F7F-F1EE-4A89-9E33-10E64038C7E2}" name="Table3" displayName="Table3" ref="S4:S5" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B9449F7F-F1EE-4A89-9E33-10E64038C7E2}" name="Table3" displayName="Table3" ref="S4:S5" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" dataCellStyle="Percent">
   <autoFilter ref="S4:S5" xr:uid="{B9449F7F-F1EE-4A89-9E33-10E64038C7E2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{EEFB88A1-114F-47A3-9703-1AFADE80F2C2}" name="Tax Rate" dataDxfId="32" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{EEFB88A1-114F-47A3-9703-1AFADE80F2C2}" name="Tax Rate" dataDxfId="48" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1393,19 +1393,19 @@
   <autoFilter ref="S29:X35" xr:uid="{2B999898-DD8A-4B5A-A7B3-AF75683FC4CB}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CD1F3E9F-0911-4C67-939E-F467E2073547}" name="Optional Addons"/>
-    <tableColumn id="2" xr3:uid="{55F83CB7-D989-4E16-A502-12C3EAA859FB}" name="Lower Body Set" dataDxfId="31">
+    <tableColumn id="2" xr3:uid="{55F83CB7-D989-4E16-A502-12C3EAA859FB}" name="Lower Body Set" dataDxfId="47">
       <calculatedColumnFormula>D20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{06B391EB-990B-4926-A197-9F33A33BAD50}" name="Core Set" dataDxfId="30">
+    <tableColumn id="3" xr3:uid="{06B391EB-990B-4926-A197-9F33A33BAD50}" name="Core Set" dataDxfId="46">
       <calculatedColumnFormula>D20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4570C0AE-F627-499E-9AC8-B57DC386F056}" name="Enhanced Core Set" dataDxfId="29">
+    <tableColumn id="4" xr3:uid="{4570C0AE-F627-499E-9AC8-B57DC386F056}" name="Enhanced Core Set" dataDxfId="45">
       <calculatedColumnFormula>D20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FB9069AA-C219-42C1-AA67-2E8E5F9EABE8}" name="Full Body Set" dataDxfId="28">
+    <tableColumn id="5" xr3:uid="{FB9069AA-C219-42C1-AA67-2E8E5F9EABE8}" name="Full Body Set" dataDxfId="44">
       <calculatedColumnFormula>D20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A94B1009-C6AC-47E2-9BE1-3AC6A7F36D5E}" name="Deluxe Tracker Set" dataDxfId="27">
+    <tableColumn id="6" xr3:uid="{A94B1009-C6AC-47E2-9BE1-3AC6A7F36D5E}" name="Deluxe Tracker Set" dataDxfId="43">
       <calculatedColumnFormula>D20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1414,42 +1414,42 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BE777F21-5F7E-4E4B-BA66-B45089E35C2A}" name="Table6" displayName="Table6" ref="S22:X27" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BE777F21-5F7E-4E4B-BA66-B45089E35C2A}" name="Table6" displayName="Table6" ref="S22:X27" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <autoFilter ref="S22:X27" xr:uid="{BE777F21-5F7E-4E4B-BA66-B45089E35C2A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E726F6E9-420E-4590-B851-07612196E2FB}" name="Assembly Cost" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{E9A0F7D3-1A39-4714-8999-E746F3794DC3}" name="Lower Body Set" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{808BC733-43EE-4E21-B368-8E1B59008315}" name="Core Set" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{CC518581-4A7B-4E11-93F3-6E9AF562DF4A}" name="Enhanced Core Set" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{969C46CE-554F-4ADC-99B4-77B362460AD8}" name="Full Body Set" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{36E35190-C3BD-491D-8815-1BE12BF88F4F}" name="Deluxe Tracker Set" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{E726F6E9-420E-4590-B851-07612196E2FB}" name="Assembly Cost" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{E9A0F7D3-1A39-4714-8999-E746F3794DC3}" name="Lower Body Set" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{808BC733-43EE-4E21-B368-8E1B59008315}" name="Core Set" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{CC518581-4A7B-4E11-93F3-6E9AF562DF4A}" name="Enhanced Core Set" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{969C46CE-554F-4ADC-99B4-77B362460AD8}" name="Full Body Set" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{36E35190-C3BD-491D-8815-1BE12BF88F4F}" name="Deluxe Tracker Set" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1937CD80-BE1B-4C67-939F-3565AB142AEB}" name="Table7" displayName="Table7" ref="A19:D29" totalsRowShown="0" headerRowBorderDxfId="15" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1937CD80-BE1B-4C67-939F-3565AB142AEB}" name="Table7" displayName="Table7" ref="A19:D29" totalsRowShown="0" headerRowBorderDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A19:D29" xr:uid="{1937CD80-BE1B-4C67-939F-3565AB142AEB}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3262E418-5713-49DA-AD70-0C8321B09A04}" name="Ancillary Components" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{8A405A15-7C4C-4AE3-9170-9C663FAB89AF}" name="38x300mm Strap" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{B59260DC-D256-4C9D-AC51-156D65EEF719}" name="38x500mm Strap" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{E65489C3-1F46-4035-8CE1-771CDA52DDB7}" name="Chest Harness" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{3262E418-5713-49DA-AD70-0C8321B09A04}" name="Ancillary Components" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{8A405A15-7C4C-4AE3-9170-9C663FAB89AF}" name="38x300mm Strap" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{B59260DC-D256-4C9D-AC51-156D65EEF719}" name="38x500mm Strap" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{E65489C3-1F46-4035-8CE1-771CDA52DDB7}" name="Chest Harness" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5CB4EC49-725A-464E-B7E5-5A1558A20F02}" name="Table79" displayName="Table79" ref="A31:E45" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5CB4EC49-725A-464E-B7E5-5A1558A20F02}" name="Table79" displayName="Table79" ref="A31:E45" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22">
   <autoFilter ref="A31:E45" xr:uid="{5CB4EC49-725A-464E-B7E5-5A1558A20F02}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{06896587-D3F2-4DE0-855E-6C92FFC78119}" name="Charging Dock Components" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B0680A55-24DD-4CA4-8565-B40C9F09C265}" name="Pogo Male" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{734E177A-4BEC-438B-B66D-EE9E42806AE3}" name="USB-C Female SMD" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{38294D5D-5885-4DF9-BCAA-920959E2E41D}" name="PCB" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{33512293-1FD2-42B9-86BB-D7FA3982F7A4}" name="Total" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{06896587-D3F2-4DE0-855E-6C92FFC78119}" name="Charging Dock Components" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{B0680A55-24DD-4CA4-8565-B40C9F09C265}" name="Pogo Male" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{734E177A-4BEC-438B-B66D-EE9E42806AE3}" name="USB-C Female SMD" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{38294D5D-5885-4DF9-BCAA-920959E2E41D}" name="PCB" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{33512293-1FD2-42B9-86BB-D7FA3982F7A4}" name="Total" dataDxfId="17">
       <calculatedColumnFormula>SUM(Table79[[#This Row],[Pogo Male]:[PCB]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1461,7 +1461,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F4A77239-5CC6-4DF4-BEE8-7839C6D245F6}" name="Table9" displayName="Table9" ref="G42:G43" totalsRowShown="0">
   <autoFilter ref="G42:G43" xr:uid="{F4A77239-5CC6-4DF4-BEE8-7839C6D245F6}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3D81F484-FB66-48E8-88F7-0E5537E0AE89}" name="Assembled Price" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{3D81F484-FB66-48E8-88F7-0E5537E0AE89}" name="Assembled Price" dataDxfId="16">
       <calculatedColumnFormula>SUM(((AA9)/60)*AA13,Table79[[#This Row],[Total]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1769,7 +1769,7 @@
   <dimension ref="A1:AA45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update BOM to reflect price of cases
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\roachslimes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9F0BDE-7969-4E3A-AA52-2B5E1857537E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD7EB40-3FD6-4E9D-B95A-5D6ECDC72F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21150" xr2:uid="{AB7D66DD-99DB-4E79-8386-D1BE3E306A87}"/>
+    <workbookView xWindow="9480" yWindow="-15870" windowWidth="29040" windowHeight="15990" xr2:uid="{AB7D66DD-99DB-4E79-8386-D1BE3E306A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
   <si>
     <t>D1 Mini</t>
   </si>
@@ -272,6 +272,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Tracker Components</t>
+  </si>
+  <si>
+    <t>Identity LEDs</t>
+  </si>
+  <si>
+    <t>3D Printed Motherboard Cases</t>
+  </si>
+  <si>
+    <t>3D Printed Daughterboard Cases</t>
   </si>
 </sst>
 </file>
@@ -457,148 +466,6 @@
   </cellStyles>
   <dxfs count="59">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
@@ -1166,6 +1033,148 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1180,11 +1189,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$R$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$R$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$R$31" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$R$32" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$R$33" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$R$34" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1323,55 +1344,256 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>390525</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D067C1F4-563E-BE97-9EC5-28F75CC15423}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>390525</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>33</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E2EA2D5-F728-C09D-912A-BE33E1F4376F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>390525</xdr:colOff>
+          <xdr:row>33</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>34</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0A4A08F-3CC8-F8A1-09A2-6D412EED80BE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B14A7224-19B0-4C1A-A967-E81C81040A40}" name="Table1" displayName="Table1" ref="A1:Q17" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B14A7224-19B0-4C1A-A967-E81C81040A40}" name="Table1" displayName="Table1" ref="A1:Q17" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A1:Q17" xr:uid="{B14A7224-19B0-4C1A-A967-E81C81040A40}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{FCE3FD92-4E2D-4CDD-8748-B2B792C3CC2B}" name=" Tracker Components" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{C043608B-6B21-430A-A486-3DBF4D729827}" name="D1 Mini" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{0FD903D3-5CF3-4816-A12C-6B81AD38D598}" name="BMI160" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{AF1B510F-1F13-4EBF-9516-C6875CCCE2FD}" name="TP4056" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{EDED6859-BC93-4D0F-9315-A40F96119E83}" name="GY-271" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{7FD415BD-A930-4596-BA13-FDA67B16B7F4}" name="SK12D07VG4 " dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{A90A17C3-9B69-4679-A66B-0EDE0EB27F40}" name="JST-PH-4P" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{FCE3FD92-4E2D-4CDD-8748-B2B792C3CC2B}" name=" Tracker Components" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{C043608B-6B21-430A-A486-3DBF4D729827}" name="D1 Mini" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{0FD903D3-5CF3-4816-A12C-6B81AD38D598}" name="BMI160" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{AF1B510F-1F13-4EBF-9516-C6875CCCE2FD}" name="TP4056" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{EDED6859-BC93-4D0F-9315-A40F96119E83}" name="GY-271" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{7FD415BD-A930-4596-BA13-FDA67B16B7F4}" name="SK12D07VG4 " dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{A90A17C3-9B69-4679-A66B-0EDE0EB27F40}" name="JST-PH-4P" dataDxfId="50"/>
     <tableColumn id="20" xr3:uid="{BB4AB17F-F072-4577-B885-41BCCBC80B3B}" name="Pogo Female"/>
-    <tableColumn id="8" xr3:uid="{A914F9A6-5FD6-48EC-9D66-948BA78CA99E}" name="B5817WS" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{38CC02EE-7A21-4150-81A5-541E2C9611DA}" name="0805 180k" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{A914F9A6-5FD6-48EC-9D66-948BA78CA99E}" name="B5817WS" dataDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{38CC02EE-7A21-4150-81A5-541E2C9611DA}" name="0805 180k" dataDxfId="48"/>
     <tableColumn id="17" xr3:uid="{D06AA3FD-469E-44E7-954C-59BA219B5A1D}" name="0806 620r"/>
     <tableColumn id="18" xr3:uid="{A346B222-7458-4A1F-8FDB-BE9A824753D5}" name="0805 LED"/>
-    <tableColumn id="10" xr3:uid="{F09ECC99-91ED-41A2-B73F-32BA143514AC}" name="803450" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{D2F40E9F-6B6D-42C4-81A7-8C00F83ACB72}" name="Wires" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{1CAFA1EE-4F95-4300-8E25-43760021F16D}" name="Motherboard" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{EBB820E5-8589-4BC4-925B-FE2B3CF62FFC}" name="Daughterboard" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{A324B42F-BFC5-4670-BD72-3FF95C7E905F}" name="Total" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{F09ECC99-91ED-41A2-B73F-32BA143514AC}" name="803450" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{D2F40E9F-6B6D-42C4-81A7-8C00F83ACB72}" name="Wires" dataDxfId="46"/>
+    <tableColumn id="12" xr3:uid="{1CAFA1EE-4F95-4300-8E25-43760021F16D}" name="Motherboard" dataDxfId="45"/>
+    <tableColumn id="13" xr3:uid="{EBB820E5-8589-4BC4-925B-FE2B3CF62FFC}" name="Daughterboard" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{A324B42F-BFC5-4670-BD72-3FF95C7E905F}" name="Total" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B93392DA-EFC7-40A8-935E-E4659A1D9845}" name="Table2" displayName="Table2" ref="S7:X20" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B93392DA-EFC7-40A8-935E-E4659A1D9845}" name="Table2" displayName="Table2" ref="S7:X20" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="S7:X20" xr:uid="{B93392DA-EFC7-40A8-935E-E4659A1D9845}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B05F922E-1AED-4BDF-AF79-C73D0E339E8C}" name=" Materials Cost" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{890D8999-0321-4F67-A5E0-25676EB95AFA}" name="Lower Body Set" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{965D71D9-87D7-40F0-AB78-E63CEFFF194C}" name="Core Set" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{A87423F7-0BA3-4F6A-B4AF-D56080DE192B}" name="Enhanced Core Set" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{15F82D2F-735C-4D15-9CD1-2FFAC68D783A}" name="Full Body Set" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{268904B6-4873-466C-AF49-A18E0B9EB3F6}" name="Deluxe Tracker Set" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{B05F922E-1AED-4BDF-AF79-C73D0E339E8C}" name=" Materials Cost" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{890D8999-0321-4F67-A5E0-25676EB95AFA}" name="Lower Body Set" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{965D71D9-87D7-40F0-AB78-E63CEFFF194C}" name="Core Set" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{A87423F7-0BA3-4F6A-B4AF-D56080DE192B}" name="Enhanced Core Set" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{15F82D2F-735C-4D15-9CD1-2FFAC68D783A}" name="Full Body Set" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{268904B6-4873-466C-AF49-A18E0B9EB3F6}" name="Deluxe Tracker Set" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B9449F7F-F1EE-4A89-9E33-10E64038C7E2}" name="Table3" displayName="Table3" ref="S4:S5" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B9449F7F-F1EE-4A89-9E33-10E64038C7E2}" name="Table3" displayName="Table3" ref="S4:S5" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" dataCellStyle="Percent">
   <autoFilter ref="S4:S5" xr:uid="{B9449F7F-F1EE-4A89-9E33-10E64038C7E2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{EEFB88A1-114F-47A3-9703-1AFADE80F2C2}" name="Tax Rate" dataDxfId="48" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{EEFB88A1-114F-47A3-9703-1AFADE80F2C2}" name="Tax Rate" dataDxfId="32" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1389,23 +1611,23 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2B999898-DD8A-4B5A-A7B3-AF75683FC4CB}" name="Table5" displayName="Table5" ref="S29:X35" totalsRowShown="0">
-  <autoFilter ref="S29:X35" xr:uid="{2B999898-DD8A-4B5A-A7B3-AF75683FC4CB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2B999898-DD8A-4B5A-A7B3-AF75683FC4CB}" name="Table5" displayName="Table5" ref="S29:X38" totalsRowShown="0">
+  <autoFilter ref="S29:X38" xr:uid="{2B999898-DD8A-4B5A-A7B3-AF75683FC4CB}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CD1F3E9F-0911-4C67-939E-F467E2073547}" name="Optional Addons"/>
-    <tableColumn id="2" xr3:uid="{55F83CB7-D989-4E16-A502-12C3EAA859FB}" name="Lower Body Set" dataDxfId="47">
+    <tableColumn id="2" xr3:uid="{55F83CB7-D989-4E16-A502-12C3EAA859FB}" name="Lower Body Set" dataDxfId="31">
       <calculatedColumnFormula>D20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{06B391EB-990B-4926-A197-9F33A33BAD50}" name="Core Set" dataDxfId="46">
+    <tableColumn id="3" xr3:uid="{06B391EB-990B-4926-A197-9F33A33BAD50}" name="Core Set" dataDxfId="30">
       <calculatedColumnFormula>D20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4570C0AE-F627-499E-9AC8-B57DC386F056}" name="Enhanced Core Set" dataDxfId="45">
+    <tableColumn id="4" xr3:uid="{4570C0AE-F627-499E-9AC8-B57DC386F056}" name="Enhanced Core Set" dataDxfId="29">
       <calculatedColumnFormula>D20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FB9069AA-C219-42C1-AA67-2E8E5F9EABE8}" name="Full Body Set" dataDxfId="44">
+    <tableColumn id="5" xr3:uid="{FB9069AA-C219-42C1-AA67-2E8E5F9EABE8}" name="Full Body Set" dataDxfId="28">
       <calculatedColumnFormula>D20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A94B1009-C6AC-47E2-9BE1-3AC6A7F36D5E}" name="Deluxe Tracker Set" dataDxfId="43">
+    <tableColumn id="6" xr3:uid="{A94B1009-C6AC-47E2-9BE1-3AC6A7F36D5E}" name="Deluxe Tracker Set" dataDxfId="27">
       <calculatedColumnFormula>D20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1414,42 +1636,42 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BE777F21-5F7E-4E4B-BA66-B45089E35C2A}" name="Table6" displayName="Table6" ref="S22:X27" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BE777F21-5F7E-4E4B-BA66-B45089E35C2A}" name="Table6" displayName="Table6" ref="S22:X27" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="S22:X27" xr:uid="{BE777F21-5F7E-4E4B-BA66-B45089E35C2A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E726F6E9-420E-4590-B851-07612196E2FB}" name="Assembly Cost" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{E9A0F7D3-1A39-4714-8999-E746F3794DC3}" name="Lower Body Set" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{808BC733-43EE-4E21-B368-8E1B59008315}" name="Core Set" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{CC518581-4A7B-4E11-93F3-6E9AF562DF4A}" name="Enhanced Core Set" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{969C46CE-554F-4ADC-99B4-77B362460AD8}" name="Full Body Set" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{36E35190-C3BD-491D-8815-1BE12BF88F4F}" name="Deluxe Tracker Set" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{E726F6E9-420E-4590-B851-07612196E2FB}" name="Assembly Cost" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{E9A0F7D3-1A39-4714-8999-E746F3794DC3}" name="Lower Body Set" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{808BC733-43EE-4E21-B368-8E1B59008315}" name="Core Set" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{CC518581-4A7B-4E11-93F3-6E9AF562DF4A}" name="Enhanced Core Set" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{969C46CE-554F-4ADC-99B4-77B362460AD8}" name="Full Body Set" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{36E35190-C3BD-491D-8815-1BE12BF88F4F}" name="Deluxe Tracker Set" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1937CD80-BE1B-4C67-939F-3565AB142AEB}" name="Table7" displayName="Table7" ref="A19:D29" totalsRowShown="0" headerRowBorderDxfId="31" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1937CD80-BE1B-4C67-939F-3565AB142AEB}" name="Table7" displayName="Table7" ref="A19:D29" totalsRowShown="0" headerRowBorderDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="A19:D29" xr:uid="{1937CD80-BE1B-4C67-939F-3565AB142AEB}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3262E418-5713-49DA-AD70-0C8321B09A04}" name="Ancillary Components" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{8A405A15-7C4C-4AE3-9170-9C663FAB89AF}" name="38x300mm Strap" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{B59260DC-D256-4C9D-AC51-156D65EEF719}" name="38x500mm Strap" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{E65489C3-1F46-4035-8CE1-771CDA52DDB7}" name="Chest Harness" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{3262E418-5713-49DA-AD70-0C8321B09A04}" name="Ancillary Components" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{8A405A15-7C4C-4AE3-9170-9C663FAB89AF}" name="38x300mm Strap" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{B59260DC-D256-4C9D-AC51-156D65EEF719}" name="38x500mm Strap" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{E65489C3-1F46-4035-8CE1-771CDA52DDB7}" name="Chest Harness" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5CB4EC49-725A-464E-B7E5-5A1558A20F02}" name="Table79" displayName="Table79" ref="A31:E45" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5CB4EC49-725A-464E-B7E5-5A1558A20F02}" name="Table79" displayName="Table79" ref="A31:E45" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
   <autoFilter ref="A31:E45" xr:uid="{5CB4EC49-725A-464E-B7E5-5A1558A20F02}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{06896587-D3F2-4DE0-855E-6C92FFC78119}" name="Charging Dock Components" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{B0680A55-24DD-4CA4-8565-B40C9F09C265}" name="Pogo Male" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{734E177A-4BEC-438B-B66D-EE9E42806AE3}" name="USB-C Female SMD" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{38294D5D-5885-4DF9-BCAA-920959E2E41D}" name="PCB" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{33512293-1FD2-42B9-86BB-D7FA3982F7A4}" name="Total" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{06896587-D3F2-4DE0-855E-6C92FFC78119}" name="Charging Dock Components" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B0680A55-24DD-4CA4-8565-B40C9F09C265}" name="Pogo Male" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{734E177A-4BEC-438B-B66D-EE9E42806AE3}" name="USB-C Female SMD" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{38294D5D-5885-4DF9-BCAA-920959E2E41D}" name="PCB" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{33512293-1FD2-42B9-86BB-D7FA3982F7A4}" name="Total" dataDxfId="1">
       <calculatedColumnFormula>SUM(Table79[[#This Row],[Pogo Male]:[PCB]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1461,7 +1683,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F4A77239-5CC6-4DF4-BEE8-7839C6D245F6}" name="Table9" displayName="Table9" ref="G42:G43" totalsRowShown="0">
   <autoFilter ref="G42:G43" xr:uid="{F4A77239-5CC6-4DF4-BEE8-7839C6D245F6}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3D81F484-FB66-48E8-88F7-0E5537E0AE89}" name="Assembled Price" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{3D81F484-FB66-48E8-88F7-0E5537E0AE89}" name="Assembled Price" dataDxfId="0">
       <calculatedColumnFormula>SUM(((AA9)/60)*AA13,Table79[[#This Row],[Total]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1768,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B5E1AB-97AA-4510-B945-E7BF9EBEF607}">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,63 +2186,63 @@
         <v>33</v>
       </c>
       <c r="B4" s="2">
-        <f>SUM(B2*B7,B3)</f>
+        <f t="shared" ref="B4:P4" si="0">SUM(B2*B7,B3)</f>
         <v>15.5</v>
       </c>
       <c r="C4" s="2">
-        <f>SUM(C2*C7,C3)</f>
+        <f t="shared" si="0"/>
         <v>12.88</v>
       </c>
       <c r="D4" s="2">
-        <f>SUM(D2*D7,D3)</f>
+        <f t="shared" si="0"/>
         <v>3.27</v>
       </c>
       <c r="E4" s="2">
-        <f>SUM(E2*E7,E3)</f>
+        <f t="shared" si="0"/>
         <v>6.9599999999999991</v>
       </c>
       <c r="F4" s="2">
-        <f>SUM(F2*F7,F3)</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="G4" s="2">
-        <f>SUM(G2*G7,G3)</f>
+        <f t="shared" si="0"/>
         <v>3.79</v>
       </c>
       <c r="H4" s="2">
-        <f>SUM(H2*H7,H3)</f>
+        <f t="shared" si="0"/>
         <v>12.93</v>
       </c>
       <c r="I4" s="2">
-        <f>SUM(I2*I7,I3)</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="J4" s="2">
-        <f>SUM(J2*J7,J3)</f>
+        <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
       <c r="K4" s="2">
-        <f>SUM(K2*K7,K3)</f>
+        <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
       <c r="L4" s="2">
-        <f>SUM(L2*L7,L3)</f>
+        <f t="shared" si="0"/>
         <v>2.4700000000000002</v>
       </c>
       <c r="M4" s="2">
-        <f>SUM(M2*M7,M3)</f>
+        <f t="shared" si="0"/>
         <v>25.99</v>
       </c>
       <c r="N4" s="2">
-        <f>SUM(N2*N7,N3)</f>
+        <f t="shared" si="0"/>
         <v>11.93</v>
       </c>
       <c r="O4" s="2">
-        <f>SUM(O2*O7,O3)</f>
+        <f t="shared" si="0"/>
         <v>3.52</v>
       </c>
       <c r="P4" s="2">
-        <f>SUM(P2*P7,P3)</f>
+        <f t="shared" si="0"/>
         <v>3.52</v>
       </c>
       <c r="Q4" s="3">
@@ -2112,59 +2334,59 @@
         <v>16.778749999999999</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" ref="C6:P6" si="0">SUM(C5,C4)</f>
+        <f t="shared" ref="C6:P6" si="1">SUM(C5,C4)</f>
         <v>13.942600000000001</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.5397750000000001</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5341999999999993</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2989999999999999</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1026749999999996</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" ref="H6" si="1">SUM(H5,H4)</f>
+        <f t="shared" ref="H6" si="2">SUM(H5,H4)</f>
         <v>13.996725</v>
       </c>
       <c r="I6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2989999999999999</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.136625</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" ref="K6" si="2">SUM(K5,K4)</f>
+        <f t="shared" ref="K6" si="3">SUM(K5,K4)</f>
         <v>1.136625</v>
       </c>
       <c r="L6" s="3">
-        <f t="shared" ref="L6" si="3">SUM(L5,L4)</f>
+        <f t="shared" ref="L6" si="4">SUM(L5,L4)</f>
         <v>2.673775</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28.134174999999999</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.914225</v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8104</v>
       </c>
       <c r="P6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8104</v>
       </c>
       <c r="Q6" s="3">
@@ -2319,63 +2541,63 @@
         <v>3</v>
       </c>
       <c r="B9" s="3">
-        <f>(B6/B7)/B8</f>
+        <f t="shared" ref="B9:P9" si="5">(B6/B7)/B8</f>
         <v>1.8643055555555554</v>
       </c>
       <c r="C9" s="3">
-        <f>(C6/C7)/C8</f>
+        <f t="shared" si="5"/>
         <v>1.1618833333333334</v>
       </c>
       <c r="D9" s="3">
-        <f>(D6/D7)/D8</f>
+        <f t="shared" si="5"/>
         <v>0.17698875</v>
       </c>
       <c r="E9" s="3">
-        <f>(E6/E7)/E8</f>
+        <f t="shared" si="5"/>
         <v>0.62784999999999991</v>
       </c>
       <c r="F9" s="3">
-        <f>(F6/F7)/F8</f>
+        <f t="shared" si="5"/>
         <v>6.4949999999999994E-2</v>
       </c>
       <c r="G9" s="3">
-        <f>(G6/G7)/G8</f>
+        <f t="shared" si="5"/>
         <v>4.1026749999999994E-2</v>
       </c>
       <c r="H9" s="3">
-        <f>(H6/H7)/H8</f>
+        <f t="shared" si="5"/>
         <v>0.69983624999999994</v>
       </c>
       <c r="I9" s="3">
-        <f>(I6/I7)/I8</f>
+        <f t="shared" si="5"/>
         <v>1.299E-2</v>
       </c>
       <c r="J9" s="3">
-        <f>(J6/J7)/J8</f>
+        <f t="shared" si="5"/>
         <v>1.136625E-2</v>
       </c>
       <c r="K9" s="3">
-        <f>(K6/K7)/K8</f>
+        <f t="shared" si="5"/>
         <v>1.136625E-2</v>
       </c>
       <c r="L9" s="3">
-        <f>(L6/L7)/L8</f>
+        <f t="shared" si="5"/>
         <v>4.4562916666666666E-3</v>
       </c>
       <c r="M9" s="3">
-        <f>(M6/M7)/M8</f>
+        <f t="shared" si="5"/>
         <v>2.8134174999999999</v>
       </c>
       <c r="N9" s="3">
-        <f>(N6/N7)/N8</f>
+        <f t="shared" si="5"/>
         <v>1.0761854166666667</v>
       </c>
       <c r="O9" s="3">
-        <f>(O6/O7)/O8</f>
+        <f t="shared" si="5"/>
         <v>0.19051999999999999</v>
       </c>
       <c r="P9" s="3">
-        <f>(P6/P7)/P8</f>
+        <f t="shared" si="5"/>
         <v>9.5259999999999997E-2</v>
       </c>
       <c r="Q9" s="3"/>
@@ -2401,7 +2623,7 @@
         <v>40</v>
       </c>
       <c r="AA9">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -2409,7 +2631,7 @@
         <v>41</v>
       </c>
       <c r="AA10">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -2576,47 +2798,47 @@
         <v>1.8643055555555554</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" ref="C14:P14" si="4">C9*C11</f>
+        <f t="shared" ref="C14:P14" si="6">C9*C11</f>
         <v>1.1618833333333334</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.17698875</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.62784999999999991</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.4949999999999994E-2</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.1026749999999994E-2</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" ref="H14" si="5">H9*H11</f>
+        <f t="shared" ref="H14" si="7">H9*H11</f>
         <v>0.69983624999999994</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.598E-2</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.136625E-2</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" ref="K14" si="6">K9*K11</f>
+        <f t="shared" ref="K14" si="8">K9*K11</f>
         <v>1.136625E-2</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" ref="L14" si="7">L9*L11</f>
+        <f t="shared" ref="L14" si="9">L9*L11</f>
         <v>4.4562916666666666E-3</v>
       </c>
       <c r="M14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.8134174999999999</v>
       </c>
       <c r="N14" s="3">
@@ -2624,11 +2846,11 @@
         <v>0</v>
       </c>
       <c r="O14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.19051999999999999</v>
       </c>
       <c r="P14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q14" s="3">
@@ -2668,59 +2890,59 @@
         <v>0</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" ref="C15:P15" si="8">C9*C12</f>
+        <f t="shared" ref="C15:P15" si="10">C9*C12</f>
         <v>1.1618833333333334</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.62784999999999991</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.1026749999999994E-2</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" ref="H15" si="9">H9*H12</f>
+        <f t="shared" ref="H15" si="11">H9*H12</f>
         <v>0</v>
       </c>
       <c r="I15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" ref="K15" si="10">K9*K12</f>
+        <f t="shared" ref="K15" si="12">K9*K12</f>
         <v>0</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" ref="L15" si="11">L9*L12</f>
+        <f t="shared" ref="L15" si="13">L9*L12</f>
         <v>0</v>
       </c>
       <c r="M15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" ref="N15" si="12">N9*N12</f>
+        <f t="shared" ref="N15" si="14">N9*N12</f>
         <v>1.0761854166666667</v>
       </c>
       <c r="O15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9.5259999999999997E-2</v>
       </c>
       <c r="Q15" s="3">
@@ -2947,23 +3169,23 @@
       </c>
       <c r="T23" s="9">
         <f>((T8*AA9)/60)*AA13</f>
-        <v>55</v>
+        <v>60.5</v>
       </c>
       <c r="U23" s="9">
         <f>((U8*AA9)/60)*AA13</f>
-        <v>55</v>
+        <v>60.5</v>
       </c>
       <c r="V23" s="9">
         <f>((V8*AA9)/60)*AA13</f>
-        <v>55</v>
+        <v>60.5</v>
       </c>
       <c r="W23" s="9">
         <f>((W8*AA9)/60)*AA13</f>
-        <v>77</v>
+        <v>84.7</v>
       </c>
       <c r="X23" s="9">
         <f>((X8*AA9)/60)*AA13</f>
-        <v>110</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
@@ -2971,7 +3193,7 @@
         <v>13</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" ref="B24" si="13">SUM(B23,B22)</f>
+        <f t="shared" ref="B24" si="15">SUM(B23,B22)</f>
         <v>6.6249000000000002</v>
       </c>
       <c r="C24" s="3">
@@ -2991,19 +3213,19 @@
       </c>
       <c r="U24" s="8">
         <f>((U9*AA10)/60)*AA13</f>
-        <v>3.6666666666666665</v>
+        <v>1.8333333333333333</v>
       </c>
       <c r="V24" s="8">
         <f>((V9*AA10)/60)*AA13</f>
-        <v>11</v>
+        <v>5.5</v>
       </c>
       <c r="W24" s="8">
         <f>((W9*AA10)/60)*AA13</f>
-        <v>11</v>
+        <v>5.5</v>
       </c>
       <c r="X24" s="8">
         <f>((X9*AA10)/60)*AA13</f>
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
@@ -3024,19 +3246,19 @@
       </c>
       <c r="T25" s="9">
         <f>SUM(T23:T24)</f>
-        <v>55</v>
+        <v>60.5</v>
       </c>
       <c r="U25" s="9">
-        <f t="shared" ref="U25:W25" si="14">SUM(U23:U24)</f>
-        <v>58.666666666666664</v>
+        <f t="shared" ref="U25:V25" si="16">SUM(U23:U24)</f>
+        <v>62.333333333333336</v>
       </c>
       <c r="V25" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>66</v>
       </c>
       <c r="W25" s="9">
-        <f t="shared" si="14"/>
-        <v>88</v>
+        <f>SUM(W23:W24)</f>
+        <v>90.2</v>
       </c>
       <c r="X25" s="9">
         <f>SUM(X23:X24)</f>
@@ -3084,11 +3306,11 @@
       </c>
       <c r="T27" s="12">
         <f>SUM(T25,T20)</f>
-        <v>98.250054652777777</v>
+        <v>103.75005465277778</v>
       </c>
       <c r="U27" s="12">
         <f>SUM(U25,U20)</f>
-        <v>106.51236681944445</v>
+        <v>110.17903348611111</v>
       </c>
       <c r="V27" s="12">
         <f>SUM(V25,V20)</f>
@@ -3096,7 +3318,7 @@
       </c>
       <c r="W27" s="12">
         <f>SUM(W25,W20)</f>
-        <v>160.15642501388891</v>
+        <v>162.3564250138889</v>
       </c>
       <c r="X27" s="12">
         <f>SUM(X25,X20)</f>
@@ -3137,30 +3359,30 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="R30" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S30" t="s">
         <v>56</v>
       </c>
       <c r="T30" s="3">
         <f>IF(R30,D27,0)</f>
-        <v>8.714125000000001</v>
+        <v>0</v>
       </c>
       <c r="U30" s="3">
         <f>IF(R30,D27,0)</f>
-        <v>8.714125000000001</v>
+        <v>0</v>
       </c>
       <c r="V30" s="3">
         <f>IF(R30,D27,0)</f>
-        <v>8.714125000000001</v>
+        <v>0</v>
       </c>
       <c r="W30" s="3">
         <f>IF(R30,D27,0)</f>
-        <v>8.714125000000001</v>
+        <v>0</v>
       </c>
       <c r="X30" s="3">
         <f>IF(R30,D27,0)</f>
-        <v>8.714125000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
@@ -3223,11 +3445,32 @@
         <f>SUM(Table79[[#This Row],[Pogo Male]:[PCB]])</f>
         <v>6.26</v>
       </c>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
+      <c r="R32" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="S32" t="s">
+        <v>72</v>
+      </c>
+      <c r="T32" s="3">
+        <f>IF(R32,((2.5/60)*AA13)*T8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U32" s="3">
+        <f>IF(R32,((2.5/60)*AA13)*U8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V32" s="3">
+        <f>IF(R32,((2.5/60)*AA13)*V8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W32" s="3">
+        <f>IF(R32,((2.5/60)*AA13)*W8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="X32" s="3">
+        <f>IF(R32,((2.5/60)*AA13)*X8,0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
@@ -3246,28 +3489,31 @@
         <f>SUM(Table79[[#This Row],[Pogo Male]:[PCB]])</f>
         <v>1.52</v>
       </c>
+      <c r="R33" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="S33" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="T33" s="3">
-        <f>SUM(T30:T31)</f>
-        <v>8.714125000000001</v>
+        <f>IF(R33,(1.69)*T8,0)</f>
+        <v>8.4499999999999993</v>
       </c>
       <c r="U33" s="3">
-        <f t="shared" ref="U33:X33" si="15">SUM(U30:U31)</f>
-        <v>8.714125000000001</v>
+        <f>IF(R33,(1.69)*U8,0)</f>
+        <v>8.4499999999999993</v>
       </c>
       <c r="V33" s="3">
-        <f t="shared" si="15"/>
-        <v>8.714125000000001</v>
+        <f>IF(R33,(1.69)*V8,0)</f>
+        <v>8.4499999999999993</v>
       </c>
       <c r="W33" s="3">
-        <f t="shared" si="15"/>
-        <v>8.714125000000001</v>
+        <f>IF(R33,(1.69)*W8,0)</f>
+        <v>11.83</v>
       </c>
       <c r="X33" s="3">
-        <f t="shared" si="15"/>
-        <v>8.714125000000001</v>
+        <f>IF(R33,(1.69)*X8,0)</f>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
@@ -3290,11 +3536,32 @@
         <f>SUM(Table79[[#This Row],[Pogo Male]:[PCB]])</f>
         <v>16.27</v>
       </c>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
+      <c r="R34" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="S34" t="s">
+        <v>74</v>
+      </c>
+      <c r="T34" s="3">
+        <f>IF(R34,(0.83)*T9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U34" s="3">
+        <f>IF(R34,(0.83)*U9,0)</f>
+        <v>0.83</v>
+      </c>
+      <c r="V34" s="3">
+        <f>IF(R34,(0.83)*V9,0)</f>
+        <v>2.4899999999999998</v>
+      </c>
+      <c r="W34" s="3">
+        <f>IF(R34,(0.83)*W9,0)</f>
+        <v>2.4899999999999998</v>
+      </c>
+      <c r="X34" s="3">
+        <f>IF(R34,(0.83)*X9,0)</f>
+        <v>4.9799999999999995</v>
+      </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
@@ -3316,29 +3583,11 @@
         <f>SUM(Table79[[#This Row],[Pogo Male]:[PCB]])</f>
         <v>1.3422750000000001</v>
       </c>
-      <c r="S35" t="s">
-        <v>67</v>
-      </c>
-      <c r="T35" s="3">
-        <f>SUM(T33,T27)</f>
-        <v>106.96417965277777</v>
-      </c>
-      <c r="U35" s="3">
-        <f t="shared" ref="U35:X35" si="16">SUM(U33,U27)</f>
-        <v>115.22649181944445</v>
-      </c>
-      <c r="V35" s="3">
-        <f t="shared" si="16"/>
-        <v>129.88921615277778</v>
-      </c>
-      <c r="W35" s="3">
-        <f t="shared" si="16"/>
-        <v>168.8705500138889</v>
-      </c>
-      <c r="X35" s="3">
-        <f t="shared" si="16"/>
-        <v>244.95900730555556</v>
-      </c>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
@@ -3360,6 +3609,29 @@
         <f>SUM(Table79[[#This Row],[Pogo Male]:[PCB]])</f>
         <v>17.612275</v>
       </c>
+      <c r="S36" t="s">
+        <v>61</v>
+      </c>
+      <c r="T36" s="3">
+        <f>SUM(T30:T34)</f>
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="U36" s="3">
+        <f t="shared" ref="U36:X36" si="17">SUM(U30:U34)</f>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="V36" s="3">
+        <f t="shared" si="17"/>
+        <v>10.94</v>
+      </c>
+      <c r="W36" s="3">
+        <f t="shared" si="17"/>
+        <v>14.32</v>
+      </c>
+      <c r="X36" s="3">
+        <f t="shared" si="17"/>
+        <v>21.88</v>
+      </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
@@ -3375,6 +3647,11 @@
         <v>1</v>
       </c>
       <c r="E37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
@@ -3390,6 +3667,29 @@
         <v>5</v>
       </c>
       <c r="E38" s="3"/>
+      <c r="S38" t="s">
+        <v>67</v>
+      </c>
+      <c r="T38" s="3">
+        <f>SUM(T36,T27)</f>
+        <v>112.20005465277778</v>
+      </c>
+      <c r="U38" s="3">
+        <f>SUM(U36,U27)</f>
+        <v>119.45903348611111</v>
+      </c>
+      <c r="V38" s="3">
+        <f>SUM(V36,V27)</f>
+        <v>132.11509115277778</v>
+      </c>
+      <c r="W38" s="3">
+        <f>SUM(W36,W27)</f>
+        <v>176.67642501388889</v>
+      </c>
+      <c r="X38" s="3">
+        <f>SUM(X36,X27)</f>
+        <v>258.12488230555556</v>
+      </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
@@ -3461,8 +3761,9 @@
       </c>
       <c r="G43" s="3">
         <f>SUM(((AA9)/60)*AA13,Table79[[#This Row],[Total]])</f>
-        <v>17.580517499999999</v>
-      </c>
+        <v>18.680517500000001</v>
+      </c>
+      <c r="T43" s="3"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
@@ -3470,6 +3771,7 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
+      <c r="T44" s="3"/>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
@@ -3499,14 +3801,15 @@
     <hyperlink ref="C19" r:id="rId17" xr:uid="{BE26F90E-F18C-4325-9898-4EF9AF31F1BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId18"/>
-  <legacyDrawing r:id="rId19"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>
+  <drawing r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId20" name="Check Box 1">
+            <control shapeId="1025" r:id="rId21" name="Check Box 1">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3528,7 +3831,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId21" name="Check Box 2">
+            <control shapeId="1026" r:id="rId22" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3548,19 +3851,85 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1027" r:id="rId23" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>17</xdr:col>
+                    <xdr:colOff>390525</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>18</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId24" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>17</xdr:col>
+                    <xdr:colOff>390525</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>18</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>33</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" r:id="rId25" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>17</xdr:col>
+                    <xdr:colOff>390525</xdr:colOff>
+                    <xdr:row>33</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>18</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>34</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
   <tableParts count="9">
-    <tablePart r:id="rId22"/>
-    <tablePart r:id="rId23"/>
-    <tablePart r:id="rId24"/>
-    <tablePart r:id="rId25"/>
     <tablePart r:id="rId26"/>
     <tablePart r:id="rId27"/>
     <tablePart r:id="rId28"/>
     <tablePart r:id="rId29"/>
     <tablePart r:id="rId30"/>
+    <tablePart r:id="rId31"/>
+    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId33"/>
+    <tablePart r:id="rId34"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finalize case designs, misc edits to readme
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\roachslimes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD7EB40-3FD6-4E9D-B95A-5D6ECDC72F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159FD6ED-5D6E-412C-957F-D756DD9911AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="-15870" windowWidth="29040" windowHeight="15990" xr2:uid="{AB7D66DD-99DB-4E79-8386-D1BE3E306A87}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21390" xr2:uid="{AB7D66DD-99DB-4E79-8386-D1BE3E306A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1367,7 +1367,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D067C1F4-563E-BE97-9EC5-28F75CC15423}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1434,7 +1434,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E2EA2D5-F728-C09D-912A-BE33E1F4376F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1501,7 +1501,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0A4A08F-3CC8-F8A1-09A2-6D412EED80BE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1990,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B5E1AB-97AA-4510-B945-E7BF9EBEF607}">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
attempt to make page wider
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\roachslimes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159FD6ED-5D6E-412C-957F-D756DD9911AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE913D5-E184-42D0-9907-FF5DFE4B9A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21390" xr2:uid="{AB7D66DD-99DB-4E79-8386-D1BE3E306A87}"/>
+    <workbookView xWindow="3630" yWindow="2370" windowWidth="57600" windowHeight="15555" xr2:uid="{AB7D66DD-99DB-4E79-8386-D1BE3E306A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1991,7 +1991,7 @@
   <dimension ref="A1:AA45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>